<commit_message>
CM Update for missing dec_id
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_CM.xlsx
+++ b/curation/draft/collection/collection_specialization_CM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B517A61-0D30-B648-863F-6AADED4A6816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EBECB1-3C08-5B43-8EE0-443F366744CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="1320" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="3520" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_CM" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="149">
   <si>
     <t>package_date</t>
   </si>
@@ -875,8 +875,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2318,6 +2318,9 @@
       <c r="M24" t="s">
         <v>103</v>
       </c>
+      <c r="N24" t="s">
+        <v>113</v>
+      </c>
       <c r="P24" t="s">
         <v>104</v>
       </c>
@@ -3743,6 +3746,9 @@
       </c>
       <c r="M47" t="s">
         <v>71</v>
+      </c>
+      <c r="N47" t="s">
+        <v>72</v>
       </c>
       <c r="P47" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
CM updated to include categories
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_CM.xlsx
+++ b/curation/draft/collection/collection_specialization_CM.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EBECB1-3C08-5B43-8EE0-443F366744CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C572AA0-B3ED-4B4D-B9C8-E3D91C0AA40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="3520" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_CM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_CM!$A$1:$AG$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_CM!$A$1:$AH$56</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="150">
   <si>
     <t>package_date</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>CMPRIORBREASTCANCER_NORMALIZED</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -873,10 +876,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AG56"/>
+  <dimension ref="A1:AH56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -886,15 +889,15 @@
     <col min="5" max="5" width="8.83203125" style="5"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
     <col min="9" max="9" width="21.1640625" customWidth="1"/>
-    <col min="11" max="11" width="39.83203125" customWidth="1"/>
-    <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" customWidth="1"/>
-    <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.83203125" customWidth="1"/>
-    <col min="31" max="31" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="39.83203125" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="16" max="16" width="22" style="2" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" customWidth="1"/>
+    <col min="32" max="32" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,76 +929,79 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>141</v>
       </c>
@@ -1011,47 +1017,47 @@
       <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>48</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>36</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>37</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>40</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>141</v>
       </c>
@@ -1067,41 +1073,41 @@
       <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="L3" t="s">
-        <v>137</v>
       </c>
       <c r="M3" t="s">
         <v>137</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" t="s">
+        <v>137</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>2</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>85</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>10</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>138</v>
       </c>
       <c r="AE3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -1123,44 +1129,44 @@
       <c r="I4" t="s">
         <v>142</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>144</v>
-      </c>
-      <c r="L4" t="s">
-        <v>44</v>
       </c>
       <c r="M4" t="s">
         <v>44</v>
       </c>
       <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
         <v>45</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>46</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>47</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>36</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>200</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>48</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>44</v>
       </c>
       <c r="AE4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1182,44 +1188,44 @@
       <c r="I5" t="s">
         <v>142</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>144</v>
-      </c>
-      <c r="L5" t="s">
-        <v>49</v>
       </c>
       <c r="M5" t="s">
         <v>49</v>
       </c>
       <c r="N5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" t="s">
         <v>50</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>51</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>47</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>36</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>200</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>48</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>49</v>
       </c>
       <c r="AE5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -1241,41 +1247,41 @@
       <c r="I6" t="s">
         <v>142</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>144</v>
-      </c>
-      <c r="L6" t="s">
-        <v>52</v>
       </c>
       <c r="M6" t="s">
         <v>52</v>
       </c>
       <c r="N6" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" t="s">
         <v>53</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>54</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>48</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>36</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>200</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>52</v>
       </c>
       <c r="AE6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>42</v>
       </c>
@@ -1297,41 +1303,41 @@
       <c r="I7" t="s">
         <v>142</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>144</v>
-      </c>
-      <c r="L7" t="s">
-        <v>55</v>
       </c>
       <c r="M7" t="s">
         <v>55</v>
       </c>
       <c r="N7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" t="s">
         <v>56</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>57</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>4</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>47</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>36</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>200</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>55</v>
       </c>
       <c r="AE7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>42</v>
       </c>
@@ -1353,38 +1359,38 @@
       <c r="I8" t="s">
         <v>142</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>144</v>
-      </c>
-      <c r="L8" t="s">
-        <v>58</v>
       </c>
       <c r="M8" t="s">
         <v>58</v>
       </c>
-      <c r="P8" t="s">
+      <c r="N8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" t="s">
         <v>59</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>5</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>48</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>36</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>100</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>60</v>
       </c>
       <c r="AE8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -1406,47 +1412,47 @@
       <c r="I9" t="s">
         <v>142</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>144</v>
-      </c>
-      <c r="L9" t="s">
-        <v>61</v>
       </c>
       <c r="M9" t="s">
         <v>61</v>
       </c>
       <c r="N9" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" t="s">
         <v>62</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>63</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>6</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>48</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>36</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>40</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>64</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>65</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>61</v>
       </c>
       <c r="AE9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -1468,47 +1474,47 @@
       <c r="I10" t="s">
         <v>142</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>144</v>
-      </c>
-      <c r="L10" t="s">
-        <v>66</v>
       </c>
       <c r="M10" t="s">
         <v>66</v>
       </c>
       <c r="N10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" t="s">
         <v>67</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>68</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>7</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>47</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>36</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>40</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>69</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>70</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>66</v>
       </c>
       <c r="AE10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>42</v>
       </c>
@@ -1530,47 +1536,47 @@
       <c r="I11" t="s">
         <v>142</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>144</v>
-      </c>
-      <c r="L11" t="s">
-        <v>71</v>
       </c>
       <c r="M11" t="s">
         <v>71</v>
       </c>
       <c r="N11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" t="s">
         <v>72</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>73</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>8</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>47</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>36</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>40</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>74</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>75</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>71</v>
       </c>
       <c r="AE11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -1592,47 +1598,47 @@
       <c r="I12" t="s">
         <v>142</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>144</v>
-      </c>
-      <c r="L12" t="s">
-        <v>76</v>
       </c>
       <c r="M12" t="s">
         <v>76</v>
       </c>
       <c r="N12" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" t="s">
         <v>77</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>78</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>9</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>47</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>36</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>40</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>79</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>80</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>76</v>
       </c>
       <c r="AE12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>42</v>
       </c>
@@ -1654,41 +1660,41 @@
       <c r="I13" t="s">
         <v>142</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>144</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>81</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>82</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>83</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>84</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>10</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>48</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>85</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>10</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>82</v>
       </c>
       <c r="AE13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>42</v>
       </c>
@@ -1710,41 +1716,41 @@
       <c r="I14" t="s">
         <v>142</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>144</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>86</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>82</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>83</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>87</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>11</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>47</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>88</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>5</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>82</v>
       </c>
       <c r="AE14" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>42</v>
       </c>
@@ -1766,50 +1772,50 @@
       <c r="I15" t="s">
         <v>142</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>144</v>
-      </c>
-      <c r="L15" t="s">
-        <v>89</v>
       </c>
       <c r="M15" t="s">
         <v>89</v>
       </c>
-      <c r="P15" t="s">
+      <c r="N15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q15" t="s">
         <v>90</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>12</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>47</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>36</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>1</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>37</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>38</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>39</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>40</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>89</v>
       </c>
       <c r="AE15" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AF15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -1831,41 +1837,41 @@
       <c r="I16" t="s">
         <v>142</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>144</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>91</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>92</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>93</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>94</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>13</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>47</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>85</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>10</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>92</v>
       </c>
       <c r="AE16" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1887,41 +1893,41 @@
       <c r="I17" t="s">
         <v>142</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>144</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>95</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>92</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>93</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>96</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>14</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>47</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>88</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>5</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>92</v>
       </c>
       <c r="AE17" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>42</v>
       </c>
@@ -1943,50 +1949,50 @@
       <c r="I18" t="s">
         <v>142</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>144</v>
-      </c>
-      <c r="L18" t="s">
-        <v>97</v>
       </c>
       <c r="M18" t="s">
         <v>97</v>
       </c>
-      <c r="P18" t="s">
+      <c r="N18" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q18" t="s">
         <v>98</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>15</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>47</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>36</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>1</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>37</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>38</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>39</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>40</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>99</v>
       </c>
       <c r="AE18" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>42</v>
       </c>
@@ -2008,44 +2014,44 @@
       <c r="I19" t="s">
         <v>142</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>146</v>
-      </c>
-      <c r="L19" t="s">
-        <v>44</v>
       </c>
       <c r="M19" t="s">
         <v>44</v>
       </c>
       <c r="N19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" t="s">
         <v>45</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>46</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>1</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>47</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>36</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>200</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>48</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>44</v>
       </c>
       <c r="AE19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>42</v>
       </c>
@@ -2067,44 +2073,44 @@
       <c r="I20" t="s">
         <v>142</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>146</v>
-      </c>
-      <c r="L20" t="s">
-        <v>49</v>
       </c>
       <c r="M20" t="s">
         <v>49</v>
       </c>
       <c r="N20" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" t="s">
         <v>50</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>51</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>2</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>47</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>36</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>200</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>48</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>49</v>
       </c>
       <c r="AE20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>42</v>
       </c>
@@ -2126,41 +2132,41 @@
       <c r="I21" t="s">
         <v>142</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>146</v>
-      </c>
-      <c r="L21" t="s">
-        <v>55</v>
       </c>
       <c r="M21" t="s">
         <v>55</v>
       </c>
       <c r="N21" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" t="s">
         <v>56</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>57</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>3</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>47</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>36</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>200</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>55</v>
       </c>
       <c r="AE21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>42</v>
       </c>
@@ -2182,41 +2188,41 @@
       <c r="I22" t="s">
         <v>142</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>146</v>
-      </c>
-      <c r="L22" t="s">
-        <v>52</v>
       </c>
       <c r="M22" t="s">
         <v>52</v>
       </c>
       <c r="N22" t="s">
+        <v>52</v>
+      </c>
+      <c r="O22" t="s">
         <v>53</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>54</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>4</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>48</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>36</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>200</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>52</v>
       </c>
       <c r="AE22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -2238,56 +2244,56 @@
       <c r="I23" t="s">
         <v>142</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>146</v>
-      </c>
-      <c r="L23" t="s">
-        <v>100</v>
       </c>
       <c r="M23" t="s">
         <v>100</v>
       </c>
       <c r="N23" t="s">
+        <v>100</v>
+      </c>
+      <c r="O23" t="s">
         <v>101</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>102</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>5</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>48</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>36</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>1</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>48</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>37</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>38</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>39</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AB23" t="s">
         <v>40</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>100</v>
       </c>
       <c r="AE23" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>42</v>
       </c>
@@ -2309,53 +2315,53 @@
       <c r="I24" t="s">
         <v>142</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>146</v>
-      </c>
-      <c r="L24" t="s">
-        <v>103</v>
       </c>
       <c r="M24" t="s">
         <v>103</v>
       </c>
       <c r="N24" t="s">
+        <v>103</v>
+      </c>
+      <c r="O24" t="s">
         <v>113</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>104</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>6</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>48</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>36</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>1</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>37</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>38</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>39</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>40</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>103</v>
       </c>
       <c r="AE24" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>42</v>
       </c>
@@ -2377,38 +2383,38 @@
       <c r="I25" t="s">
         <v>142</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>146</v>
-      </c>
-      <c r="L25" t="s">
-        <v>58</v>
       </c>
       <c r="M25" t="s">
         <v>58</v>
       </c>
-      <c r="P25" t="s">
+      <c r="N25" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q25" t="s">
         <v>59</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>7</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>48</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>36</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>100</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>60</v>
       </c>
       <c r="AE25" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>42</v>
       </c>
@@ -2430,47 +2436,47 @@
       <c r="I26" t="s">
         <v>142</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>146</v>
-      </c>
-      <c r="L26" t="s">
-        <v>61</v>
       </c>
       <c r="M26" t="s">
         <v>61</v>
       </c>
       <c r="N26" t="s">
+        <v>61</v>
+      </c>
+      <c r="O26" t="s">
         <v>62</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>63</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>8</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>48</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>36</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>40</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>64</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>65</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>61</v>
       </c>
       <c r="AE26" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>42</v>
       </c>
@@ -2492,47 +2498,47 @@
       <c r="I27" t="s">
         <v>142</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>146</v>
-      </c>
-      <c r="L27" t="s">
-        <v>66</v>
       </c>
       <c r="M27" t="s">
         <v>66</v>
       </c>
       <c r="N27" t="s">
+        <v>66</v>
+      </c>
+      <c r="O27" t="s">
         <v>67</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>68</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>9</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>47</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>36</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>40</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>69</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>70</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>66</v>
       </c>
       <c r="AE27" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>42</v>
       </c>
@@ -2554,47 +2560,47 @@
       <c r="I28" t="s">
         <v>142</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>146</v>
-      </c>
-      <c r="L28" t="s">
-        <v>71</v>
       </c>
       <c r="M28" t="s">
         <v>71</v>
       </c>
       <c r="N28" t="s">
+        <v>71</v>
+      </c>
+      <c r="O28" t="s">
         <v>72</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>73</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>10</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>47</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>36</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>40</v>
       </c>
-      <c r="W28" t="s">
+      <c r="X28" t="s">
         <v>74</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Y28" t="s">
         <v>75</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>71</v>
       </c>
       <c r="AE28" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -2616,47 +2622,47 @@
       <c r="I29" t="s">
         <v>142</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>146</v>
-      </c>
-      <c r="L29" t="s">
-        <v>76</v>
       </c>
       <c r="M29" t="s">
         <v>76</v>
       </c>
       <c r="N29" t="s">
+        <v>76</v>
+      </c>
+      <c r="O29" t="s">
         <v>77</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>78</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>11</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>47</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>36</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>40</v>
       </c>
-      <c r="W29" t="s">
+      <c r="X29" t="s">
         <v>79</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Y29" t="s">
         <v>80</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>76</v>
       </c>
       <c r="AE29" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>42</v>
       </c>
@@ -2678,41 +2684,41 @@
       <c r="I30" t="s">
         <v>142</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>146</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>81</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>82</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>83</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>84</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>12</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>48</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>85</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>10</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>82</v>
       </c>
       <c r="AE30" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>42</v>
       </c>
@@ -2734,41 +2740,41 @@
       <c r="I31" t="s">
         <v>142</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>146</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>86</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>82</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>83</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>87</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>13</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>47</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>88</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>5</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>82</v>
       </c>
       <c r="AE31" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>42</v>
       </c>
@@ -2790,50 +2796,50 @@
       <c r="I32" t="s">
         <v>142</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>146</v>
-      </c>
-      <c r="L32" t="s">
-        <v>89</v>
       </c>
       <c r="M32" t="s">
         <v>89</v>
       </c>
-      <c r="P32" t="s">
+      <c r="N32" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q32" t="s">
         <v>90</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>14</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>47</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>36</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>1</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>37</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>38</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>39</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AB32" t="s">
         <v>40</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>89</v>
       </c>
       <c r="AE32" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>42</v>
       </c>
@@ -2855,41 +2861,41 @@
       <c r="I33" t="s">
         <v>142</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>146</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>91</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>92</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>93</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>94</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <v>15</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>47</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>85</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>10</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>92</v>
       </c>
       <c r="AE33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>42</v>
       </c>
@@ -2911,41 +2917,41 @@
       <c r="I34" t="s">
         <v>142</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>146</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>95</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>92</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>93</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>96</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>16</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>47</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>88</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>5</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>92</v>
       </c>
       <c r="AE34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>42</v>
       </c>
@@ -2967,50 +2973,50 @@
       <c r="I35" t="s">
         <v>142</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>146</v>
-      </c>
-      <c r="L35" t="s">
-        <v>97</v>
       </c>
       <c r="M35" t="s">
         <v>97</v>
       </c>
-      <c r="P35" t="s">
+      <c r="N35" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q35" t="s">
         <v>98</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>17</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>47</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>36</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <v>1</v>
       </c>
-      <c r="W35" t="s">
+      <c r="X35" t="s">
         <v>37</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
         <v>38</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Z35" t="s">
         <v>39</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AB35" t="s">
         <v>40</v>
-      </c>
-      <c r="AD35" t="s">
-        <v>99</v>
       </c>
       <c r="AE35" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>42</v>
       </c>
@@ -3032,47 +3038,47 @@
       <c r="I36" t="s">
         <v>142</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>147</v>
-      </c>
-      <c r="L36" t="s">
-        <v>44</v>
       </c>
       <c r="M36" t="s">
         <v>44</v>
       </c>
       <c r="N36" t="s">
+        <v>44</v>
+      </c>
+      <c r="O36" t="s">
         <v>45</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>46</v>
       </c>
-      <c r="Q36">
+      <c r="R36">
         <v>1</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>47</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>36</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>200</v>
       </c>
-      <c r="V36" t="s">
+      <c r="W36" t="s">
         <v>48</v>
       </c>
-      <c r="AB36" t="s">
+      <c r="AC36" t="s">
         <v>106</v>
       </c>
-      <c r="AD36" t="s">
+      <c r="AE36" t="s">
         <v>44</v>
       </c>
-      <c r="AE36" t="s">
+      <c r="AF36" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>42</v>
       </c>
@@ -3094,47 +3100,47 @@
       <c r="I37" t="s">
         <v>142</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>147</v>
-      </c>
-      <c r="L37" t="s">
-        <v>55</v>
       </c>
       <c r="M37" t="s">
         <v>55</v>
       </c>
       <c r="N37" t="s">
+        <v>55</v>
+      </c>
+      <c r="O37" t="s">
         <v>56</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>57</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <v>2</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>47</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>36</v>
       </c>
-      <c r="T37">
+      <c r="U37">
         <v>200</v>
       </c>
-      <c r="V37" t="s">
+      <c r="W37" t="s">
         <v>48</v>
       </c>
-      <c r="AB37" t="s">
+      <c r="AC37" t="s">
         <v>107</v>
       </c>
-      <c r="AD37" t="s">
+      <c r="AE37" t="s">
         <v>55</v>
       </c>
-      <c r="AE37" t="s">
+      <c r="AF37" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>42</v>
       </c>
@@ -3156,47 +3162,47 @@
       <c r="I38" t="s">
         <v>142</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>147</v>
-      </c>
-      <c r="L38" t="s">
-        <v>108</v>
       </c>
       <c r="M38" t="s">
         <v>108</v>
       </c>
-      <c r="P38" t="s">
+      <c r="N38" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q38" t="s">
         <v>109</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <v>3</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>48</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>36</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <v>20</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>110</v>
       </c>
       <c r="Z38" t="s">
         <v>110</v>
       </c>
       <c r="AA38" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB38" t="s">
         <v>40</v>
-      </c>
-      <c r="AD38" t="s">
-        <v>108</v>
       </c>
       <c r="AE38" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>42</v>
       </c>
@@ -3218,50 +3224,50 @@
       <c r="I39" t="s">
         <v>142</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>147</v>
-      </c>
-      <c r="L39" t="s">
-        <v>52</v>
       </c>
       <c r="M39" t="s">
         <v>52</v>
       </c>
       <c r="N39" t="s">
+        <v>52</v>
+      </c>
+      <c r="O39" t="s">
         <v>53</v>
       </c>
-      <c r="P39" t="s">
+      <c r="Q39" t="s">
         <v>54</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <v>4</v>
       </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>48</v>
       </c>
-      <c r="S39" t="s">
+      <c r="T39" t="s">
         <v>36</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>200</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Z39" t="s">
         <v>111</v>
       </c>
-      <c r="Z39" t="s">
+      <c r="AA39" t="s">
         <v>112</v>
       </c>
-      <c r="AA39" t="s">
+      <c r="AB39" t="s">
         <v>40</v>
-      </c>
-      <c r="AD39" t="s">
-        <v>52</v>
       </c>
       <c r="AE39" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>42</v>
       </c>
@@ -3283,56 +3289,56 @@
       <c r="I40" t="s">
         <v>142</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>147</v>
-      </c>
-      <c r="L40" t="s">
-        <v>100</v>
       </c>
       <c r="M40" t="s">
         <v>100</v>
       </c>
       <c r="N40" t="s">
+        <v>100</v>
+      </c>
+      <c r="O40" t="s">
         <v>101</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>102</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <v>5</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>48</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>36</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>1</v>
       </c>
-      <c r="V40" t="s">
+      <c r="W40" t="s">
         <v>48</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
         <v>37</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>38</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>39</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AB40" t="s">
         <v>40</v>
-      </c>
-      <c r="AD40" t="s">
-        <v>100</v>
       </c>
       <c r="AE40" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>42</v>
       </c>
@@ -3354,56 +3360,56 @@
       <c r="I41" t="s">
         <v>142</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>147</v>
-      </c>
-      <c r="L41" t="s">
-        <v>103</v>
       </c>
       <c r="M41" t="s">
         <v>103</v>
       </c>
       <c r="N41" t="s">
+        <v>103</v>
+      </c>
+      <c r="O41" t="s">
         <v>113</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>104</v>
       </c>
-      <c r="Q41">
+      <c r="R41">
         <v>6</v>
       </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>48</v>
       </c>
-      <c r="S41" t="s">
+      <c r="T41" t="s">
         <v>36</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <v>1</v>
       </c>
-      <c r="V41" t="s">
+      <c r="W41" t="s">
         <v>48</v>
       </c>
-      <c r="W41" t="s">
+      <c r="X41" t="s">
         <v>37</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Y41" t="s">
         <v>38</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Z41" t="s">
         <v>39</v>
       </c>
-      <c r="AA41" t="s">
+      <c r="AB41" t="s">
         <v>40</v>
-      </c>
-      <c r="AD41" t="s">
-        <v>103</v>
       </c>
       <c r="AE41" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>42</v>
       </c>
@@ -3425,53 +3431,53 @@
       <c r="I42" t="s">
         <v>142</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>147</v>
-      </c>
-      <c r="L42" t="s">
-        <v>114</v>
       </c>
       <c r="M42" t="s">
         <v>114</v>
       </c>
-      <c r="P42" t="s">
+      <c r="N42" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q42" t="s">
         <v>115</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <v>7</v>
       </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
         <v>47</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>36</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <v>200</v>
       </c>
-      <c r="W42" t="s">
+      <c r="X42" t="s">
         <v>116</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Y42" t="s">
         <v>117</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>118</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="AA42" t="s">
         <v>119</v>
       </c>
-      <c r="AA42" t="s">
+      <c r="AB42" t="s">
         <v>40</v>
-      </c>
-      <c r="AD42" t="s">
-        <v>114</v>
       </c>
       <c r="AE42" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -3493,53 +3499,53 @@
       <c r="I43" t="s">
         <v>142</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>147</v>
-      </c>
-      <c r="L43" t="s">
-        <v>120</v>
       </c>
       <c r="M43" t="s">
         <v>120</v>
       </c>
-      <c r="P43" t="s">
+      <c r="N43" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q43" t="s">
         <v>121</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <v>8</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>47</v>
       </c>
-      <c r="S43" t="s">
+      <c r="T43" t="s">
         <v>36</v>
       </c>
-      <c r="T43">
+      <c r="U43">
         <v>200</v>
       </c>
-      <c r="W43" t="s">
+      <c r="X43" t="s">
         <v>122</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" t="s">
         <v>123</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>124</v>
       </c>
-      <c r="Z43" t="s">
+      <c r="AA43" t="s">
         <v>125</v>
       </c>
-      <c r="AA43" t="s">
+      <c r="AB43" t="s">
         <v>40</v>
-      </c>
-      <c r="AD43" t="s">
-        <v>120</v>
       </c>
       <c r="AE43" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>42</v>
       </c>
@@ -3561,38 +3567,38 @@
       <c r="I44" t="s">
         <v>142</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>147</v>
-      </c>
-      <c r="L44" t="s">
-        <v>58</v>
       </c>
       <c r="M44" t="s">
         <v>58</v>
       </c>
-      <c r="P44" t="s">
+      <c r="N44" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q44" t="s">
         <v>59</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <v>9</v>
       </c>
-      <c r="R44" t="s">
+      <c r="S44" t="s">
         <v>48</v>
       </c>
-      <c r="S44" t="s">
+      <c r="T44" t="s">
         <v>36</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>100</v>
-      </c>
-      <c r="AD44" t="s">
-        <v>60</v>
       </c>
       <c r="AE44" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>42</v>
       </c>
@@ -3614,47 +3620,47 @@
       <c r="I45" t="s">
         <v>142</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>147</v>
-      </c>
-      <c r="L45" t="s">
-        <v>61</v>
       </c>
       <c r="M45" t="s">
         <v>61</v>
       </c>
       <c r="N45" t="s">
+        <v>61</v>
+      </c>
+      <c r="O45" t="s">
         <v>62</v>
       </c>
-      <c r="P45" t="s">
+      <c r="Q45" t="s">
         <v>63</v>
       </c>
-      <c r="Q45">
+      <c r="R45">
         <v>10</v>
       </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
         <v>48</v>
       </c>
-      <c r="S45" t="s">
+      <c r="T45" t="s">
         <v>36</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>40</v>
       </c>
-      <c r="W45" t="s">
+      <c r="X45" t="s">
         <v>64</v>
       </c>
-      <c r="X45" t="s">
+      <c r="Y45" t="s">
         <v>65</v>
-      </c>
-      <c r="AD45" t="s">
-        <v>61</v>
       </c>
       <c r="AE45" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>42</v>
       </c>
@@ -3676,47 +3682,47 @@
       <c r="I46" t="s">
         <v>142</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>147</v>
-      </c>
-      <c r="L46" t="s">
-        <v>66</v>
       </c>
       <c r="M46" t="s">
         <v>66</v>
       </c>
       <c r="N46" t="s">
+        <v>66</v>
+      </c>
+      <c r="O46" t="s">
         <v>67</v>
       </c>
-      <c r="P46" t="s">
+      <c r="Q46" t="s">
         <v>68</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <v>11</v>
       </c>
-      <c r="R46" t="s">
+      <c r="S46" t="s">
         <v>47</v>
       </c>
-      <c r="S46" t="s">
+      <c r="T46" t="s">
         <v>36</v>
       </c>
-      <c r="T46">
+      <c r="U46">
         <v>40</v>
       </c>
-      <c r="W46" t="s">
+      <c r="X46" t="s">
         <v>69</v>
       </c>
-      <c r="X46" t="s">
+      <c r="Y46" t="s">
         <v>70</v>
-      </c>
-      <c r="AD46" t="s">
-        <v>66</v>
       </c>
       <c r="AE46" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>42</v>
       </c>
@@ -3738,47 +3744,47 @@
       <c r="I47" t="s">
         <v>142</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>147</v>
-      </c>
-      <c r="L47" t="s">
-        <v>71</v>
       </c>
       <c r="M47" t="s">
         <v>71</v>
       </c>
       <c r="N47" t="s">
+        <v>71</v>
+      </c>
+      <c r="O47" t="s">
         <v>72</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>73</v>
       </c>
-      <c r="Q47">
+      <c r="R47">
         <v>12</v>
       </c>
-      <c r="R47" t="s">
+      <c r="S47" t="s">
         <v>47</v>
       </c>
-      <c r="S47" t="s">
+      <c r="T47" t="s">
         <v>36</v>
       </c>
-      <c r="T47">
+      <c r="U47">
         <v>40</v>
       </c>
-      <c r="W47" t="s">
+      <c r="X47" t="s">
         <v>74</v>
       </c>
-      <c r="X47" t="s">
+      <c r="Y47" t="s">
         <v>75</v>
-      </c>
-      <c r="AD47" t="s">
-        <v>71</v>
       </c>
       <c r="AE47" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>42</v>
       </c>
@@ -3800,38 +3806,38 @@
       <c r="I48" t="s">
         <v>142</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>147</v>
-      </c>
-      <c r="L48" t="s">
-        <v>126</v>
       </c>
       <c r="M48" t="s">
         <v>126</v>
       </c>
-      <c r="P48" t="s">
+      <c r="N48" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q48" t="s">
         <v>127</v>
       </c>
-      <c r="Q48">
+      <c r="R48">
         <v>13</v>
       </c>
-      <c r="R48" t="s">
+      <c r="S48" t="s">
         <v>47</v>
       </c>
-      <c r="S48" t="s">
+      <c r="T48" t="s">
         <v>36</v>
       </c>
-      <c r="T48">
+      <c r="U48">
         <v>200</v>
-      </c>
-      <c r="AD48" t="s">
-        <v>126</v>
       </c>
       <c r="AE48" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>42</v>
       </c>
@@ -3853,47 +3859,47 @@
       <c r="I49" t="s">
         <v>142</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>147</v>
-      </c>
-      <c r="L49" t="s">
-        <v>76</v>
       </c>
       <c r="M49" t="s">
         <v>76</v>
       </c>
       <c r="N49" t="s">
+        <v>76</v>
+      </c>
+      <c r="O49" t="s">
         <v>77</v>
       </c>
-      <c r="P49" t="s">
+      <c r="Q49" t="s">
         <v>78</v>
       </c>
-      <c r="Q49">
+      <c r="R49">
         <v>14</v>
       </c>
-      <c r="R49" t="s">
+      <c r="S49" t="s">
         <v>47</v>
       </c>
-      <c r="S49" t="s">
+      <c r="T49" t="s">
         <v>36</v>
       </c>
-      <c r="T49">
+      <c r="U49">
         <v>200</v>
       </c>
-      <c r="W49" t="s">
+      <c r="X49" t="s">
         <v>79</v>
       </c>
-      <c r="X49" t="s">
+      <c r="Y49" t="s">
         <v>80</v>
-      </c>
-      <c r="AD49" t="s">
-        <v>76</v>
       </c>
       <c r="AE49" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>42</v>
       </c>
@@ -3915,41 +3921,41 @@
       <c r="I50" t="s">
         <v>142</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>147</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>81</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>82</v>
       </c>
-      <c r="N50" t="s">
+      <c r="O50" t="s">
         <v>83</v>
       </c>
-      <c r="P50" t="s">
+      <c r="Q50" t="s">
         <v>84</v>
       </c>
-      <c r="Q50">
+      <c r="R50">
         <v>15</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>48</v>
       </c>
-      <c r="S50" t="s">
+      <c r="T50" t="s">
         <v>85</v>
       </c>
-      <c r="T50">
+      <c r="U50">
         <v>10</v>
-      </c>
-      <c r="AD50" t="s">
-        <v>82</v>
       </c>
       <c r="AE50" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="51" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>42</v>
       </c>
@@ -3971,41 +3977,41 @@
       <c r="I51" t="s">
         <v>142</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>147</v>
       </c>
-      <c r="L51" t="s">
+      <c r="M51" t="s">
         <v>86</v>
       </c>
-      <c r="M51" t="s">
+      <c r="N51" t="s">
         <v>82</v>
       </c>
-      <c r="N51" t="s">
+      <c r="O51" t="s">
         <v>83</v>
       </c>
-      <c r="P51" t="s">
+      <c r="Q51" t="s">
         <v>87</v>
       </c>
-      <c r="Q51">
+      <c r="R51">
         <v>16</v>
       </c>
-      <c r="R51" t="s">
+      <c r="S51" t="s">
         <v>47</v>
       </c>
-      <c r="S51" t="s">
+      <c r="T51" t="s">
         <v>88</v>
       </c>
-      <c r="T51">
+      <c r="U51">
         <v>5</v>
-      </c>
-      <c r="AD51" t="s">
-        <v>82</v>
       </c>
       <c r="AE51" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>42</v>
       </c>
@@ -4027,50 +4033,50 @@
       <c r="I52" t="s">
         <v>142</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>147</v>
-      </c>
-      <c r="L52" t="s">
-        <v>89</v>
       </c>
       <c r="M52" t="s">
         <v>89</v>
       </c>
-      <c r="P52" t="s">
+      <c r="N52" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q52" t="s">
         <v>90</v>
       </c>
-      <c r="Q52">
+      <c r="R52">
         <v>17</v>
       </c>
-      <c r="R52" t="s">
+      <c r="S52" t="s">
         <v>47</v>
       </c>
-      <c r="S52" t="s">
+      <c r="T52" t="s">
         <v>36</v>
       </c>
-      <c r="T52">
+      <c r="U52">
         <v>1</v>
       </c>
-      <c r="W52" t="s">
+      <c r="X52" t="s">
         <v>37</v>
       </c>
-      <c r="X52" t="s">
+      <c r="Y52" t="s">
         <v>38</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>39</v>
       </c>
-      <c r="AA52" t="s">
+      <c r="AB52" t="s">
         <v>40</v>
-      </c>
-      <c r="AD52" t="s">
-        <v>89</v>
       </c>
       <c r="AE52" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="53" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>42</v>
       </c>
@@ -4092,41 +4098,41 @@
       <c r="I53" t="s">
         <v>142</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>147</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
         <v>91</v>
       </c>
-      <c r="M53" t="s">
+      <c r="N53" t="s">
         <v>92</v>
       </c>
-      <c r="N53" t="s">
+      <c r="O53" t="s">
         <v>93</v>
       </c>
-      <c r="P53" t="s">
+      <c r="Q53" t="s">
         <v>94</v>
       </c>
-      <c r="Q53">
+      <c r="R53">
         <v>18</v>
       </c>
-      <c r="R53" t="s">
+      <c r="S53" t="s">
         <v>47</v>
       </c>
-      <c r="S53" t="s">
+      <c r="T53" t="s">
         <v>85</v>
       </c>
-      <c r="T53">
+      <c r="U53">
         <v>10</v>
-      </c>
-      <c r="AD53" t="s">
-        <v>92</v>
       </c>
       <c r="AE53" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="54" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>42</v>
       </c>
@@ -4148,41 +4154,41 @@
       <c r="I54" t="s">
         <v>142</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>147</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>95</v>
       </c>
-      <c r="M54" t="s">
+      <c r="N54" t="s">
         <v>92</v>
       </c>
-      <c r="N54" t="s">
+      <c r="O54" t="s">
         <v>93</v>
       </c>
-      <c r="P54" t="s">
+      <c r="Q54" t="s">
         <v>96</v>
       </c>
-      <c r="Q54">
+      <c r="R54">
         <v>19</v>
       </c>
-      <c r="R54" t="s">
+      <c r="S54" t="s">
         <v>47</v>
       </c>
-      <c r="S54" t="s">
+      <c r="T54" t="s">
         <v>88</v>
       </c>
-      <c r="T54">
+      <c r="U54">
         <v>5</v>
-      </c>
-      <c r="AD54" t="s">
-        <v>92</v>
       </c>
       <c r="AE54" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="55" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>42</v>
       </c>
@@ -4204,50 +4210,50 @@
       <c r="I55" t="s">
         <v>142</v>
       </c>
-      <c r="K55" t="s">
+      <c r="L55" t="s">
         <v>147</v>
-      </c>
-      <c r="L55" t="s">
-        <v>97</v>
       </c>
       <c r="M55" t="s">
         <v>97</v>
       </c>
-      <c r="P55" t="s">
+      <c r="N55" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q55" t="s">
         <v>98</v>
       </c>
-      <c r="Q55">
+      <c r="R55">
         <v>20</v>
       </c>
-      <c r="R55" t="s">
+      <c r="S55" t="s">
         <v>47</v>
       </c>
-      <c r="S55" t="s">
+      <c r="T55" t="s">
         <v>36</v>
       </c>
-      <c r="T55">
+      <c r="U55">
         <v>1</v>
       </c>
-      <c r="W55" t="s">
+      <c r="X55" t="s">
         <v>37</v>
       </c>
-      <c r="X55" t="s">
+      <c r="Y55" t="s">
         <v>38</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>39</v>
       </c>
-      <c r="AA55" t="s">
+      <c r="AB55" t="s">
         <v>40</v>
-      </c>
-      <c r="AD55" t="s">
-        <v>99</v>
       </c>
       <c r="AE55" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="56" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AF55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>42</v>
       </c>
@@ -4269,48 +4275,48 @@
       <c r="I56" t="s">
         <v>142</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>147</v>
-      </c>
-      <c r="L56" t="s">
-        <v>128</v>
       </c>
       <c r="M56" t="s">
         <v>128</v>
       </c>
-      <c r="P56" t="s">
+      <c r="N56" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q56" t="s">
         <v>129</v>
       </c>
-      <c r="Q56">
+      <c r="R56">
         <v>21</v>
       </c>
-      <c r="R56" t="s">
+      <c r="S56" t="s">
         <v>47</v>
       </c>
-      <c r="S56" t="s">
+      <c r="T56" t="s">
         <v>36</v>
       </c>
-      <c r="T56">
+      <c r="U56">
         <v>200</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>130</v>
       </c>
-      <c r="Z56" t="s">
+      <c r="AA56" t="s">
         <v>131</v>
       </c>
-      <c r="AA56" t="s">
+      <c r="AB56" t="s">
         <v>40</v>
-      </c>
-      <c r="AD56" t="s">
-        <v>128</v>
       </c>
       <c r="AE56" t="s">
         <v>128</v>
       </c>
+      <c r="AF56" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG56" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:AH56" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="C53630"/>

</xml_diff>

<commit_message>
added derivation columns (blank) and updated mapping for Prior and Ongoing
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_CM.xlsx
+++ b/curation/draft/collection/collection_specialization_CM.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C572AA0-B3ED-4B4D-B9C8-E3D91C0AA40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21702868-256C-1748-BD7E-97B82846C1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="780" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_CM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_CM!$A$1:$AH$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_CM!$A$1:$AJ$56</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="155">
   <si>
     <t>package_date</t>
   </si>
@@ -322,9 +322,6 @@
     <t>Ongoing</t>
   </si>
   <si>
-    <t>CMENRF;CMENRTPT</t>
-  </si>
-  <si>
     <t>CMPRESP</t>
   </si>
   <si>
@@ -473,13 +470,41 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <r>
+      <t>CMENRF;CMENRTPT;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CMENTPT</t>
+    </r>
+  </si>
+  <si>
+    <t>[NOT SUBMITTED];CMENRF;CMENRTPT;CMENTPT</t>
+  </si>
+  <si>
+    <t>CMSTRF;CMSTRTPT;CMSTTPT</t>
+  </si>
+  <si>
+    <t>[NOT SUBMITTED];CMSTRF;CMSTRTPT;CMSTTPT</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +530,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -557,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -573,6 +603,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,10 +908,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AH56"/>
+  <dimension ref="A1:AJ56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -887,17 +919,22 @@
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="5"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="34.6640625" customWidth="1"/>
     <col min="9" max="9" width="21.1640625" customWidth="1"/>
     <col min="12" max="12" width="39.83203125" customWidth="1"/>
     <col min="13" max="13" width="21.5" customWidth="1"/>
     <col min="14" max="14" width="14.83203125" customWidth="1"/>
     <col min="16" max="16" width="22" style="2" customWidth="1"/>
-    <col min="17" max="17" width="16.83203125" customWidth="1"/>
-    <col min="32" max="32" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="34.5" customWidth="1"/>
+    <col min="23" max="23" width="13.5" customWidth="1"/>
+    <col min="25" max="25" width="14.83203125" customWidth="1"/>
+    <col min="28" max="28" width="32.83203125" customWidth="1"/>
+    <col min="29" max="29" width="39.6640625" customWidth="1"/>
+    <col min="33" max="33" width="32.5" customWidth="1"/>
+    <col min="34" max="34" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +966,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -968,57 +1005,63 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
@@ -1041,52 +1084,52 @@
       <c r="U2">
         <v>1</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>37</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="M3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="M3" t="s">
-        <v>137</v>
-      </c>
-      <c r="N3" t="s">
-        <v>137</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="R3" s="2">
         <v>2</v>
@@ -1100,14 +1143,14 @@
       <c r="U3">
         <v>10</v>
       </c>
-      <c r="AE3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AG3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -1115,22 +1158,22 @@
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G4" t="s">
         <v>33</v>
       </c>
       <c r="H4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+      <c r="L4" t="s">
         <v>143</v>
-      </c>
-      <c r="I4" t="s">
-        <v>142</v>
-      </c>
-      <c r="L4" t="s">
-        <v>144</v>
       </c>
       <c r="M4" t="s">
         <v>44</v>
@@ -1159,14 +1202,14 @@
       <c r="W4" t="s">
         <v>48</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>44</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1174,22 +1217,22 @@
         <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
       </c>
       <c r="H5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" t="s">
         <v>143</v>
-      </c>
-      <c r="I5" t="s">
-        <v>142</v>
-      </c>
-      <c r="L5" t="s">
-        <v>144</v>
       </c>
       <c r="M5" t="s">
         <v>49</v>
@@ -1218,14 +1261,14 @@
       <c r="W5" t="s">
         <v>48</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>49</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AH5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -1233,22 +1276,22 @@
         <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
       </c>
       <c r="H6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="L6" t="s">
         <v>143</v>
-      </c>
-      <c r="I6" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" t="s">
-        <v>144</v>
       </c>
       <c r="M6" t="s">
         <v>52</v>
@@ -1274,14 +1317,14 @@
       <c r="U6">
         <v>200</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>52</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>42</v>
       </c>
@@ -1289,22 +1332,22 @@
         <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G7" t="s">
         <v>33</v>
       </c>
       <c r="H7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="L7" t="s">
         <v>143</v>
-      </c>
-      <c r="I7" t="s">
-        <v>142</v>
-      </c>
-      <c r="L7" t="s">
-        <v>144</v>
       </c>
       <c r="M7" t="s">
         <v>55</v>
@@ -1330,14 +1373,14 @@
       <c r="U7">
         <v>200</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>55</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>42</v>
       </c>
@@ -1345,22 +1388,22 @@
         <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
         <v>33</v>
       </c>
       <c r="H8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L8" t="s">
         <v>143</v>
-      </c>
-      <c r="I8" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" t="s">
-        <v>144</v>
       </c>
       <c r="M8" t="s">
         <v>58</v>
@@ -1383,14 +1426,14 @@
       <c r="U8">
         <v>100</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>60</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -1398,22 +1441,22 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G9" t="s">
         <v>33</v>
       </c>
       <c r="H9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="L9" t="s">
         <v>143</v>
-      </c>
-      <c r="I9" t="s">
-        <v>142</v>
-      </c>
-      <c r="L9" t="s">
-        <v>144</v>
       </c>
       <c r="M9" t="s">
         <v>61</v>
@@ -1439,20 +1482,23 @@
       <c r="U9">
         <v>40</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Z9" t="s">
         <v>64</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AA9" t="s">
         <v>65</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AD9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG9" t="s">
         <v>61</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AH9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -1460,22 +1506,22 @@
         <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" t="s">
         <v>33</v>
       </c>
       <c r="H10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L10" t="s">
         <v>143</v>
-      </c>
-      <c r="I10" t="s">
-        <v>142</v>
-      </c>
-      <c r="L10" t="s">
-        <v>144</v>
       </c>
       <c r="M10" t="s">
         <v>66</v>
@@ -1501,20 +1547,23 @@
       <c r="U10">
         <v>40</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Z10" t="s">
         <v>69</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AA10" t="s">
         <v>70</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AD10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG10" t="s">
         <v>66</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>42</v>
       </c>
@@ -1522,22 +1571,22 @@
         <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G11" t="s">
         <v>33</v>
       </c>
       <c r="H11" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L11" t="s">
         <v>143</v>
-      </c>
-      <c r="I11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L11" t="s">
-        <v>144</v>
       </c>
       <c r="M11" t="s">
         <v>71</v>
@@ -1563,20 +1612,23 @@
       <c r="U11">
         <v>40</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z11" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AA11" t="s">
         <v>75</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AD11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG11" t="s">
         <v>71</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AH11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -1584,22 +1636,22 @@
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G12" t="s">
         <v>33</v>
       </c>
       <c r="H12" t="s">
+        <v>142</v>
+      </c>
+      <c r="I12" t="s">
+        <v>141</v>
+      </c>
+      <c r="L12" t="s">
         <v>143</v>
-      </c>
-      <c r="I12" t="s">
-        <v>142</v>
-      </c>
-      <c r="L12" t="s">
-        <v>144</v>
       </c>
       <c r="M12" t="s">
         <v>76</v>
@@ -1625,20 +1677,23 @@
       <c r="U12">
         <v>40</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Z12" t="s">
         <v>79</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AA12" t="s">
         <v>80</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AD12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG12" t="s">
         <v>76</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AH12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>42</v>
       </c>
@@ -1646,22 +1701,22 @@
         <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" t="s">
         <v>33</v>
       </c>
       <c r="H13" t="s">
+        <v>142</v>
+      </c>
+      <c r="I13" t="s">
+        <v>141</v>
+      </c>
+      <c r="L13" t="s">
         <v>143</v>
-      </c>
-      <c r="I13" t="s">
-        <v>142</v>
-      </c>
-      <c r="L13" t="s">
-        <v>144</v>
       </c>
       <c r="M13" t="s">
         <v>81</v>
@@ -1687,14 +1742,14 @@
       <c r="U13">
         <v>10</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AG13" t="s">
         <v>82</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AH13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>42</v>
       </c>
@@ -1702,22 +1757,22 @@
         <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" t="s">
         <v>33</v>
       </c>
       <c r="H14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I14" t="s">
+        <v>141</v>
+      </c>
+      <c r="L14" t="s">
         <v>143</v>
-      </c>
-      <c r="I14" t="s">
-        <v>142</v>
-      </c>
-      <c r="L14" t="s">
-        <v>144</v>
       </c>
       <c r="M14" t="s">
         <v>86</v>
@@ -1743,14 +1798,14 @@
       <c r="U14">
         <v>5</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AG14" t="s">
         <v>82</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AH14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>42</v>
       </c>
@@ -1758,22 +1813,22 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
         <v>33</v>
       </c>
       <c r="H15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I15" t="s">
+        <v>141</v>
+      </c>
+      <c r="L15" t="s">
         <v>143</v>
-      </c>
-      <c r="I15" t="s">
-        <v>142</v>
-      </c>
-      <c r="L15" t="s">
-        <v>144</v>
       </c>
       <c r="M15" t="s">
         <v>89</v>
@@ -1796,26 +1851,26 @@
       <c r="U15">
         <v>1</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Z15" t="s">
         <v>37</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="AA15" t="s">
         <v>38</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AB15" t="s">
         <v>39</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AD15" t="s">
         <v>40</v>
       </c>
-      <c r="AE15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AG15" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -1823,22 +1878,22 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" t="s">
         <v>33</v>
       </c>
       <c r="H16" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" t="s">
+        <v>141</v>
+      </c>
+      <c r="L16" t="s">
         <v>143</v>
-      </c>
-      <c r="I16" t="s">
-        <v>142</v>
-      </c>
-      <c r="L16" t="s">
-        <v>144</v>
       </c>
       <c r="M16" t="s">
         <v>91</v>
@@ -1864,14 +1919,14 @@
       <c r="U16">
         <v>10</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AG16" t="s">
         <v>92</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AH16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1879,22 +1934,22 @@
         <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G17" t="s">
         <v>33</v>
       </c>
       <c r="H17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L17" t="s">
         <v>143</v>
-      </c>
-      <c r="I17" t="s">
-        <v>142</v>
-      </c>
-      <c r="L17" t="s">
-        <v>144</v>
       </c>
       <c r="M17" t="s">
         <v>95</v>
@@ -1920,14 +1975,14 @@
       <c r="U17">
         <v>5</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AG17" t="s">
         <v>92</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AH17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>42</v>
       </c>
@@ -1935,22 +1990,22 @@
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
         <v>33</v>
       </c>
       <c r="H18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I18" t="s">
+        <v>141</v>
+      </c>
+      <c r="L18" t="s">
         <v>143</v>
-      </c>
-      <c r="I18" t="s">
-        <v>142</v>
-      </c>
-      <c r="L18" t="s">
-        <v>144</v>
       </c>
       <c r="M18" t="s">
         <v>97</v>
@@ -1973,49 +2028,49 @@
       <c r="U18">
         <v>1</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Z18" t="s">
         <v>37</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="AA18" t="s">
         <v>38</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AB18" t="s">
         <v>39</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AD18" t="s">
         <v>40</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AG18" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH18" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
         <v>99</v>
       </c>
-      <c r="AF18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>100</v>
-      </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G19" t="s">
         <v>33</v>
       </c>
       <c r="H19" t="s">
+        <v>144</v>
+      </c>
+      <c r="I19" t="s">
+        <v>141</v>
+      </c>
+      <c r="L19" t="s">
         <v>145</v>
-      </c>
-      <c r="I19" t="s">
-        <v>142</v>
-      </c>
-      <c r="L19" t="s">
-        <v>146</v>
       </c>
       <c r="M19" t="s">
         <v>44</v>
@@ -2044,37 +2099,37 @@
       <c r="W19" t="s">
         <v>48</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AG19" t="s">
         <v>44</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AH19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G20" t="s">
         <v>33</v>
       </c>
       <c r="H20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" t="s">
+        <v>141</v>
+      </c>
+      <c r="L20" t="s">
         <v>145</v>
-      </c>
-      <c r="I20" t="s">
-        <v>142</v>
-      </c>
-      <c r="L20" t="s">
-        <v>146</v>
       </c>
       <c r="M20" t="s">
         <v>49</v>
@@ -2103,37 +2158,37 @@
       <c r="W20" t="s">
         <v>48</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AG20" t="s">
         <v>49</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AH20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G21" t="s">
         <v>33</v>
       </c>
       <c r="H21" t="s">
+        <v>144</v>
+      </c>
+      <c r="I21" t="s">
+        <v>141</v>
+      </c>
+      <c r="L21" t="s">
         <v>145</v>
-      </c>
-      <c r="I21" t="s">
-        <v>142</v>
-      </c>
-      <c r="L21" t="s">
-        <v>146</v>
       </c>
       <c r="M21" t="s">
         <v>55</v>
@@ -2159,37 +2214,37 @@
       <c r="U21">
         <v>200</v>
       </c>
-      <c r="AE21" t="s">
+      <c r="AG21" t="s">
         <v>55</v>
       </c>
-      <c r="AF21" t="s">
+      <c r="AH21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
       </c>
       <c r="H22" t="s">
+        <v>144</v>
+      </c>
+      <c r="I22" t="s">
+        <v>141</v>
+      </c>
+      <c r="L22" t="s">
         <v>145</v>
-      </c>
-      <c r="I22" t="s">
-        <v>142</v>
-      </c>
-      <c r="L22" t="s">
-        <v>146</v>
       </c>
       <c r="M22" t="s">
         <v>52</v>
@@ -2215,49 +2270,49 @@
       <c r="U22">
         <v>200</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AG22" t="s">
         <v>52</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AH22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>42</v>
       </c>
       <c r="C23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" t="s">
+        <v>141</v>
+      </c>
+      <c r="L23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M23" t="s">
+        <v>99</v>
+      </c>
+      <c r="N23" t="s">
+        <v>99</v>
+      </c>
+      <c r="O23" t="s">
         <v>100</v>
       </c>
-      <c r="D23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" t="s">
-        <v>145</v>
-      </c>
-      <c r="I23" t="s">
-        <v>142</v>
-      </c>
-      <c r="L23" t="s">
-        <v>146</v>
-      </c>
-      <c r="M23" t="s">
-        <v>100</v>
-      </c>
-      <c r="N23" t="s">
-        <v>100</v>
-      </c>
-      <c r="O23" t="s">
+      <c r="Q23" t="s">
         <v>101</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>102</v>
       </c>
       <c r="R23">
         <v>5</v>
@@ -2274,61 +2329,61 @@
       <c r="W23" t="s">
         <v>48</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Z23" t="s">
         <v>37</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="AA23" t="s">
         <v>38</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="AB23" t="s">
         <v>39</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AD23" t="s">
         <v>40</v>
       </c>
-      <c r="AE23" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG23" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
       </c>
       <c r="H24" t="s">
+        <v>144</v>
+      </c>
+      <c r="I24" t="s">
+        <v>141</v>
+      </c>
+      <c r="L24" t="s">
         <v>145</v>
       </c>
-      <c r="I24" t="s">
-        <v>142</v>
-      </c>
-      <c r="L24" t="s">
-        <v>146</v>
-      </c>
       <c r="M24" t="s">
+        <v>102</v>
+      </c>
+      <c r="N24" t="s">
+        <v>102</v>
+      </c>
+      <c r="O24" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q24" t="s">
         <v>103</v>
-      </c>
-      <c r="N24" t="s">
-        <v>103</v>
-      </c>
-      <c r="O24" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>104</v>
       </c>
       <c r="R24">
         <v>6</v>
@@ -2342,49 +2397,49 @@
       <c r="U24">
         <v>1</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Z24" t="s">
         <v>37</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="AA24" t="s">
         <v>38</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AB24" t="s">
         <v>39</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AD24" t="s">
         <v>40</v>
       </c>
-      <c r="AE24" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG24" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G25" t="s">
         <v>33</v>
       </c>
       <c r="H25" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" t="s">
+        <v>141</v>
+      </c>
+      <c r="L25" t="s">
         <v>145</v>
-      </c>
-      <c r="I25" t="s">
-        <v>142</v>
-      </c>
-      <c r="L25" t="s">
-        <v>146</v>
       </c>
       <c r="M25" t="s">
         <v>58</v>
@@ -2407,37 +2462,37 @@
       <c r="U25">
         <v>100</v>
       </c>
-      <c r="AE25" t="s">
+      <c r="AG25" t="s">
         <v>60</v>
       </c>
-      <c r="AF25" t="s">
+      <c r="AH25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" t="s">
         <v>33</v>
       </c>
       <c r="H26" t="s">
+        <v>144</v>
+      </c>
+      <c r="I26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L26" t="s">
         <v>145</v>
-      </c>
-      <c r="I26" t="s">
-        <v>142</v>
-      </c>
-      <c r="L26" t="s">
-        <v>146</v>
       </c>
       <c r="M26" t="s">
         <v>61</v>
@@ -2463,43 +2518,46 @@
       <c r="U26">
         <v>40</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Z26" t="s">
         <v>64</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="AA26" t="s">
         <v>65</v>
       </c>
-      <c r="AE26" t="s">
+      <c r="AD26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG26" t="s">
         <v>61</v>
       </c>
-      <c r="AF26" t="s">
+      <c r="AH26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G27" t="s">
         <v>33</v>
       </c>
       <c r="H27" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" t="s">
+        <v>141</v>
+      </c>
+      <c r="L27" t="s">
         <v>145</v>
-      </c>
-      <c r="I27" t="s">
-        <v>142</v>
-      </c>
-      <c r="L27" t="s">
-        <v>146</v>
       </c>
       <c r="M27" t="s">
         <v>66</v>
@@ -2525,43 +2583,46 @@
       <c r="U27">
         <v>40</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Z27" t="s">
         <v>69</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="AA27" t="s">
         <v>70</v>
       </c>
-      <c r="AE27" t="s">
+      <c r="AD27" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG27" t="s">
         <v>66</v>
       </c>
-      <c r="AF27" t="s">
+      <c r="AH27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" t="s">
         <v>33</v>
       </c>
       <c r="H28" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" t="s">
+        <v>141</v>
+      </c>
+      <c r="L28" t="s">
         <v>145</v>
-      </c>
-      <c r="I28" t="s">
-        <v>142</v>
-      </c>
-      <c r="L28" t="s">
-        <v>146</v>
       </c>
       <c r="M28" t="s">
         <v>71</v>
@@ -2587,43 +2648,46 @@
       <c r="U28">
         <v>40</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Z28" t="s">
         <v>74</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="AA28" t="s">
         <v>75</v>
       </c>
-      <c r="AE28" t="s">
+      <c r="AD28" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG28" t="s">
         <v>71</v>
       </c>
-      <c r="AF28" t="s">
+      <c r="AH28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G29" t="s">
         <v>33</v>
       </c>
       <c r="H29" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" t="s">
+        <v>141</v>
+      </c>
+      <c r="L29" t="s">
         <v>145</v>
-      </c>
-      <c r="I29" t="s">
-        <v>142</v>
-      </c>
-      <c r="L29" t="s">
-        <v>146</v>
       </c>
       <c r="M29" t="s">
         <v>76</v>
@@ -2649,43 +2713,46 @@
       <c r="U29">
         <v>40</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Z29" t="s">
         <v>79</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="AA29" t="s">
         <v>80</v>
       </c>
-      <c r="AE29" t="s">
+      <c r="AD29" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG29" t="s">
         <v>76</v>
       </c>
-      <c r="AF29" t="s">
+      <c r="AH29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
         <v>33</v>
       </c>
       <c r="H30" t="s">
+        <v>144</v>
+      </c>
+      <c r="I30" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" t="s">
         <v>145</v>
-      </c>
-      <c r="I30" t="s">
-        <v>142</v>
-      </c>
-      <c r="L30" t="s">
-        <v>146</v>
       </c>
       <c r="M30" t="s">
         <v>81</v>
@@ -2711,37 +2778,37 @@
       <c r="U30">
         <v>10</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AG30" t="s">
         <v>82</v>
       </c>
-      <c r="AF30" t="s">
+      <c r="AH30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G31" t="s">
         <v>33</v>
       </c>
       <c r="H31" t="s">
+        <v>144</v>
+      </c>
+      <c r="I31" t="s">
+        <v>141</v>
+      </c>
+      <c r="L31" t="s">
         <v>145</v>
-      </c>
-      <c r="I31" t="s">
-        <v>142</v>
-      </c>
-      <c r="L31" t="s">
-        <v>146</v>
       </c>
       <c r="M31" t="s">
         <v>86</v>
@@ -2767,37 +2834,37 @@
       <c r="U31">
         <v>5</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AG31" t="s">
         <v>82</v>
       </c>
-      <c r="AF31" t="s">
+      <c r="AH31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G32" t="s">
         <v>33</v>
       </c>
       <c r="H32" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" t="s">
+        <v>141</v>
+      </c>
+      <c r="L32" t="s">
         <v>145</v>
-      </c>
-      <c r="I32" t="s">
-        <v>142</v>
-      </c>
-      <c r="L32" t="s">
-        <v>146</v>
       </c>
       <c r="M32" t="s">
         <v>89</v>
@@ -2820,49 +2887,49 @@
       <c r="U32">
         <v>1</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Z32" t="s">
         <v>37</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="AA32" t="s">
         <v>38</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AB32" t="s">
         <v>39</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AD32" t="s">
         <v>40</v>
       </c>
-      <c r="AE32" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG32" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
       </c>
       <c r="H33" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33" t="s">
+        <v>141</v>
+      </c>
+      <c r="L33" t="s">
         <v>145</v>
-      </c>
-      <c r="I33" t="s">
-        <v>142</v>
-      </c>
-      <c r="L33" t="s">
-        <v>146</v>
       </c>
       <c r="M33" t="s">
         <v>91</v>
@@ -2888,37 +2955,37 @@
       <c r="U33">
         <v>10</v>
       </c>
-      <c r="AE33" t="s">
+      <c r="AG33" t="s">
         <v>92</v>
       </c>
-      <c r="AF33" t="s">
+      <c r="AH33" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G34" t="s">
         <v>33</v>
       </c>
       <c r="H34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I34" t="s">
+        <v>141</v>
+      </c>
+      <c r="L34" t="s">
         <v>145</v>
-      </c>
-      <c r="I34" t="s">
-        <v>142</v>
-      </c>
-      <c r="L34" t="s">
-        <v>146</v>
       </c>
       <c r="M34" t="s">
         <v>95</v>
@@ -2944,37 +3011,37 @@
       <c r="U34">
         <v>5</v>
       </c>
-      <c r="AE34" t="s">
+      <c r="AG34" t="s">
         <v>92</v>
       </c>
-      <c r="AF34" t="s">
+      <c r="AH34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G35" t="s">
         <v>33</v>
       </c>
       <c r="H35" t="s">
+        <v>144</v>
+      </c>
+      <c r="I35" t="s">
+        <v>141</v>
+      </c>
+      <c r="L35" t="s">
         <v>145</v>
-      </c>
-      <c r="I35" t="s">
-        <v>142</v>
-      </c>
-      <c r="L35" t="s">
-        <v>146</v>
       </c>
       <c r="M35" t="s">
         <v>97</v>
@@ -2997,49 +3064,49 @@
       <c r="U35">
         <v>1</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Z35" t="s">
         <v>37</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="AA35" t="s">
         <v>38</v>
       </c>
-      <c r="Z35" t="s">
+      <c r="AB35" t="s">
         <v>39</v>
       </c>
-      <c r="AB35" t="s">
+      <c r="AD35" t="s">
         <v>40</v>
       </c>
-      <c r="AE35" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG35" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH35" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G36" t="s">
         <v>33</v>
       </c>
       <c r="H36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M36" t="s">
         <v>44</v>
@@ -3068,40 +3135,40 @@
       <c r="W36" t="s">
         <v>48</v>
       </c>
-      <c r="AC36" t="s">
-        <v>106</v>
-      </c>
       <c r="AE36" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG36" t="s">
         <v>44</v>
       </c>
-      <c r="AF36" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AH36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G37" t="s">
         <v>33</v>
       </c>
       <c r="H37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M37" t="s">
         <v>55</v>
@@ -3130,49 +3197,49 @@
       <c r="W37" t="s">
         <v>48</v>
       </c>
-      <c r="AC37" t="s">
+      <c r="AE37" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" t="s">
+        <v>147</v>
+      </c>
+      <c r="I38" t="s">
+        <v>141</v>
+      </c>
+      <c r="L38" t="s">
+        <v>146</v>
+      </c>
+      <c r="M38" t="s">
         <v>107</v>
       </c>
-      <c r="AE37" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38" t="s">
-        <v>33</v>
-      </c>
-      <c r="H38" t="s">
-        <v>148</v>
-      </c>
-      <c r="I38" t="s">
-        <v>142</v>
-      </c>
-      <c r="L38" t="s">
-        <v>147</v>
-      </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q38" t="s">
         <v>108</v>
-      </c>
-      <c r="N38" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>109</v>
       </c>
       <c r="R38">
         <v>3</v>
@@ -3186,46 +3253,46 @@
       <c r="U38">
         <v>20</v>
       </c>
-      <c r="Z38" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>110</v>
-      </c>
       <c r="AB38" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD38" t="s">
         <v>40</v>
       </c>
-      <c r="AE38" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG38" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G39" t="s">
         <v>33</v>
       </c>
       <c r="H39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M39" t="s">
         <v>52</v>
@@ -3251,58 +3318,58 @@
       <c r="U39">
         <v>200</v>
       </c>
-      <c r="Z39" t="s">
+      <c r="AB39" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC39" t="s">
         <v>111</v>
       </c>
-      <c r="AA39" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB39" t="s">
+      <c r="AD39" t="s">
         <v>40</v>
       </c>
-      <c r="AE39" t="s">
+      <c r="AG39" t="s">
         <v>52</v>
       </c>
-      <c r="AF39" t="s">
+      <c r="AH39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40" t="s">
         <v>33</v>
       </c>
       <c r="H40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M40" t="s">
+        <v>99</v>
+      </c>
+      <c r="N40" t="s">
+        <v>99</v>
+      </c>
+      <c r="O40" t="s">
         <v>100</v>
       </c>
-      <c r="N40" t="s">
-        <v>100</v>
-      </c>
-      <c r="O40" t="s">
+      <c r="Q40" t="s">
         <v>101</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>102</v>
       </c>
       <c r="R40">
         <v>5</v>
@@ -3319,61 +3386,61 @@
       <c r="W40" t="s">
         <v>48</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Z40" t="s">
         <v>37</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="AA40" t="s">
         <v>38</v>
       </c>
-      <c r="Z40" t="s">
+      <c r="AB40" t="s">
         <v>39</v>
       </c>
-      <c r="AB40" t="s">
+      <c r="AD40" t="s">
         <v>40</v>
       </c>
-      <c r="AE40" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG40" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G41" t="s">
         <v>33</v>
       </c>
       <c r="H41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M41" t="s">
+        <v>102</v>
+      </c>
+      <c r="N41" t="s">
+        <v>102</v>
+      </c>
+      <c r="O41" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q41" t="s">
         <v>103</v>
-      </c>
-      <c r="N41" t="s">
-        <v>103</v>
-      </c>
-      <c r="O41" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>104</v>
       </c>
       <c r="R41">
         <v>6</v>
@@ -3390,58 +3457,58 @@
       <c r="W41" t="s">
         <v>48</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Z41" t="s">
         <v>37</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="AA41" t="s">
         <v>38</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="AB41" t="s">
         <v>39</v>
       </c>
-      <c r="AB41" t="s">
+      <c r="AD41" t="s">
         <v>40</v>
       </c>
-      <c r="AE41" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG41" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G42" t="s">
         <v>33</v>
       </c>
       <c r="H42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M42" t="s">
+        <v>113</v>
+      </c>
+      <c r="N42" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q42" t="s">
         <v>114</v>
-      </c>
-      <c r="N42" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>115</v>
       </c>
       <c r="R42">
         <v>7</v>
@@ -3455,61 +3522,61 @@
       <c r="U42">
         <v>200</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Z42" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA42" t="s">
         <v>116</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="AB42" t="s">
         <v>117</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="AC42" t="s">
         <v>118</v>
       </c>
-      <c r="AA42" t="s">
+      <c r="AD42" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" t="s">
+        <v>147</v>
+      </c>
+      <c r="I43" t="s">
+        <v>141</v>
+      </c>
+      <c r="L43" t="s">
+        <v>146</v>
+      </c>
+      <c r="M43" t="s">
         <v>119</v>
       </c>
-      <c r="AB42" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE42" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>105</v>
-      </c>
-      <c r="D43" t="s">
-        <v>132</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G43" t="s">
-        <v>33</v>
-      </c>
-      <c r="H43" t="s">
-        <v>148</v>
-      </c>
-      <c r="I43" t="s">
-        <v>142</v>
-      </c>
-      <c r="L43" t="s">
-        <v>147</v>
-      </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q43" t="s">
         <v>120</v>
-      </c>
-      <c r="N43" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>121</v>
       </c>
       <c r="R43">
         <v>8</v>
@@ -3523,52 +3590,52 @@
       <c r="U43">
         <v>200</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Z43" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA43" t="s">
         <v>122</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="AB43" t="s">
         <v>123</v>
       </c>
-      <c r="Z43" t="s">
+      <c r="AC43" t="s">
         <v>124</v>
       </c>
-      <c r="AA43" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB43" t="s">
+      <c r="AD43" t="s">
         <v>40</v>
       </c>
-      <c r="AE43" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG43" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G44" t="s">
         <v>33</v>
       </c>
       <c r="H44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M44" t="s">
         <v>58</v>
@@ -3591,37 +3658,37 @@
       <c r="U44">
         <v>100</v>
       </c>
-      <c r="AE44" t="s">
+      <c r="AG44" t="s">
         <v>60</v>
       </c>
-      <c r="AF44" t="s">
+      <c r="AH44" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G45" t="s">
         <v>33</v>
       </c>
       <c r="H45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M45" t="s">
         <v>61</v>
@@ -3647,43 +3714,46 @@
       <c r="U45">
         <v>40</v>
       </c>
-      <c r="X45" t="s">
+      <c r="Z45" t="s">
         <v>64</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="AA45" t="s">
         <v>65</v>
       </c>
-      <c r="AE45" t="s">
+      <c r="AD45" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG45" t="s">
         <v>61</v>
       </c>
-      <c r="AF45" t="s">
+      <c r="AH45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G46" t="s">
         <v>33</v>
       </c>
       <c r="H46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M46" t="s">
         <v>66</v>
@@ -3709,43 +3779,46 @@
       <c r="U46">
         <v>40</v>
       </c>
-      <c r="X46" t="s">
+      <c r="Z46" t="s">
         <v>69</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="AA46" t="s">
         <v>70</v>
       </c>
-      <c r="AE46" t="s">
+      <c r="AD46" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG46" t="s">
         <v>66</v>
       </c>
-      <c r="AF46" t="s">
+      <c r="AH46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G47" t="s">
         <v>33</v>
       </c>
       <c r="H47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M47" t="s">
         <v>71</v>
@@ -3771,52 +3844,55 @@
       <c r="U47">
         <v>40</v>
       </c>
-      <c r="X47" t="s">
+      <c r="Z47" t="s">
         <v>74</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="AA47" t="s">
         <v>75</v>
       </c>
-      <c r="AE47" t="s">
+      <c r="AD47" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG47" t="s">
         <v>71</v>
       </c>
-      <c r="AF47" t="s">
+      <c r="AH47" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G48" t="s">
         <v>33</v>
       </c>
       <c r="H48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M48" t="s">
+        <v>125</v>
+      </c>
+      <c r="N48" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q48" t="s">
         <v>126</v>
-      </c>
-      <c r="N48" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>127</v>
       </c>
       <c r="R48">
         <v>13</v>
@@ -3830,37 +3906,37 @@
       <c r="U48">
         <v>200</v>
       </c>
-      <c r="AE48" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG48" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G49" t="s">
         <v>33</v>
       </c>
       <c r="H49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M49" t="s">
         <v>76</v>
@@ -3886,43 +3962,46 @@
       <c r="U49">
         <v>200</v>
       </c>
-      <c r="X49" t="s">
+      <c r="Z49" t="s">
         <v>79</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="AA49" t="s">
         <v>80</v>
       </c>
-      <c r="AE49" t="s">
+      <c r="AD49" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG49" t="s">
         <v>76</v>
       </c>
-      <c r="AF49" t="s">
+      <c r="AH49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G50" t="s">
         <v>33</v>
       </c>
       <c r="H50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M50" t="s">
         <v>81</v>
@@ -3948,37 +4027,37 @@
       <c r="U50">
         <v>10</v>
       </c>
-      <c r="AE50" t="s">
+      <c r="AG50" t="s">
         <v>82</v>
       </c>
-      <c r="AF50" t="s">
+      <c r="AH50" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G51" t="s">
         <v>33</v>
       </c>
       <c r="H51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M51" t="s">
         <v>86</v>
@@ -4004,37 +4083,37 @@
       <c r="U51">
         <v>5</v>
       </c>
-      <c r="AE51" t="s">
+      <c r="AG51" t="s">
         <v>82</v>
       </c>
-      <c r="AF51" t="s">
+      <c r="AH51" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G52" t="s">
         <v>33</v>
       </c>
       <c r="H52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M52" t="s">
         <v>89</v>
@@ -4057,49 +4136,49 @@
       <c r="U52">
         <v>1</v>
       </c>
-      <c r="X52" t="s">
+      <c r="Z52" t="s">
         <v>37</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="AA52" t="s">
         <v>38</v>
       </c>
-      <c r="Z52" t="s">
+      <c r="AB52" t="s">
         <v>39</v>
       </c>
-      <c r="AB52" t="s">
+      <c r="AD52" t="s">
         <v>40</v>
       </c>
-      <c r="AE52" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF52" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG52" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH52" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G53" t="s">
         <v>33</v>
       </c>
       <c r="H53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M53" t="s">
         <v>91</v>
@@ -4125,37 +4204,37 @@
       <c r="U53">
         <v>10</v>
       </c>
-      <c r="AE53" t="s">
+      <c r="AG53" t="s">
         <v>92</v>
       </c>
-      <c r="AF53" t="s">
+      <c r="AH53" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G54" t="s">
         <v>33</v>
       </c>
       <c r="H54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L54" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M54" t="s">
         <v>95</v>
@@ -4181,37 +4260,37 @@
       <c r="U54">
         <v>5</v>
       </c>
-      <c r="AE54" t="s">
+      <c r="AG54" t="s">
         <v>92</v>
       </c>
-      <c r="AF54" t="s">
+      <c r="AH54" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D55" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G55" t="s">
         <v>33</v>
       </c>
       <c r="H55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M55" t="s">
         <v>97</v>
@@ -4234,58 +4313,58 @@
       <c r="U55">
         <v>1</v>
       </c>
-      <c r="X55" t="s">
+      <c r="Z55" t="s">
         <v>37</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="AA55" t="s">
         <v>38</v>
       </c>
-      <c r="Z55" t="s">
+      <c r="AB55" t="s">
         <v>39</v>
       </c>
-      <c r="AB55" t="s">
+      <c r="AD55" t="s">
         <v>40</v>
       </c>
-      <c r="AE55" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF55" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="56" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AG55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH55" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>42</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D56" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G56" t="s">
         <v>33</v>
       </c>
       <c r="H56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M56" t="s">
+        <v>127</v>
+      </c>
+      <c r="N56" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q56" t="s">
         <v>128</v>
-      </c>
-      <c r="N56" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>129</v>
       </c>
       <c r="R56">
         <v>21</v>
@@ -4299,24 +4378,24 @@
       <c r="U56">
         <v>200</v>
       </c>
-      <c r="Z56" t="s">
+      <c r="AB56" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC56" t="s">
         <v>130</v>
       </c>
-      <c r="AA56" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB56" t="s">
+      <c r="AD56" t="s">
         <v>40</v>
       </c>
-      <c r="AE56" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF56" t="s">
-        <v>128</v>
+      <c r="AG56" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH56" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH56" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:AJ56" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="C53630"/>

</xml_diff>